<commit_message>
Load properties from json
</commit_message>
<xml_diff>
--- a/BNP_template.xlsx
+++ b/BNP_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="677" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CRA" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="94">
-  <si>
-    <t>{{d2si.logo}}</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="292">
+  <si>
+    <t>{{company.logo}}</t>
   </si>
   <si>
     <t>COMPTE RENDU D'ACTIVITE MENSUEL</t>
@@ -35,7 +35,7 @@
     <t>Correspondant technique</t>
   </si>
   <si>
-    <t>{{d2si.consultant.name}}</t>
+    <t>{{company.employee.name}}</t>
   </si>
   <si>
     <t>{{client.name}}</t>
@@ -44,13 +44,13 @@
     <t>Fournisseur</t>
   </si>
   <si>
-    <t>{{d2si.administrative.name}}</t>
+    <t>{{company.administrative.name}}</t>
   </si>
   <si>
     <t>CONTRAT N°</t>
   </si>
   <si>
-    <t>{{d2si.contract}}</t>
+    <t>{{company.employee.contract}}</t>
   </si>
   <si>
     <t>PRESTATIONS</t>
@@ -260,9 +260,207 @@
     <t>AM</t>
   </si>
   <si>
+    <t>{{worked_days.1.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.2.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.3.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.4.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.5.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.6.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.7.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.8.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.9.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.10.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.11.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.12.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.13.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.14.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.15.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.16.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.17.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.18.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.19.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.20.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.21.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.22.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.23.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.24.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.25.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.26.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.27.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.28.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.29.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.30.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.31.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.32.AM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.sum.AM}}</t>
+  </si>
+  <si>
     <t>PM</t>
   </si>
   <si>
+    <t>{{worked_days.1.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.2.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.3.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.4.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.5.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.6.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.7.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.8.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.9.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.10.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.11.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.12.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.13.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.14.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.15.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.16.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.17.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.18.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.19.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.20.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.21.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.22.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.23.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.24.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.25.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.26.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.27.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.28.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.29.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.30.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.31.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.32.PM}}</t>
+  </si>
+  <si>
+    <t>{{worked_days.sum.PM}}</t>
+  </si>
+  <si>
     <t>les jours cochés correspondent à l'exécution des Prestations (matin et après midi)</t>
   </si>
   <si>
@@ -272,13 +470,409 @@
     <t>SAMEDI, DIMANCHE, JOURS FERIES</t>
   </si>
   <si>
+    <t>{{extra_worked_days.1.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.2.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.3.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.4.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.5.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.6.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.7.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.8.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.9.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.10.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.11.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.12.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.13.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.14.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.15.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.16.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.17.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.18.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.19.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.20.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.21.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.22.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.23.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.24.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.25.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.26.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.27.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.28.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.29.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.30.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.31.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.32.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.sum.AM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.1.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.2.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.3.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.4.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.5.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.6.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.7.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.8.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.9.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.10.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.11.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.12.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.13.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.14.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.15.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.16.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.17.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.18.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.19.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.20.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.21.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.22.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.23.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.24.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.25.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.26.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.27.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.28.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.29.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.30.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.31.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.32.PM}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.sum.PM}}</t>
+  </si>
+  <si>
     <t>NUITS</t>
   </si>
   <si>
     <t>22h-02h</t>
   </si>
   <si>
+    <t>{{extra_worked_days.1.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.2.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.3.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.4.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.5.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.6.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.7.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.8.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.9.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.10.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.11.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.12.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.13.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.14.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.15.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.16.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.17.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.18.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.19.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.20.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.21.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.22.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.23.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.24.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.25.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.26.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.27.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.28.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.29.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.30.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.31.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.32.NIGHT}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.sum.NIGHT}}</t>
+  </si>
+  <si>
     <t>02h-06h</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.1.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.2.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.3.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.4.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.5.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.6.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.7.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.8.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.9.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.10.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.11.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.12.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.13.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.14.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.15.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.16.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.17.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.18.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.19.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.20.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.21.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.22.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.23.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.24.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.25.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.26.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.27.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.28.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.29.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.30.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.31.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.32.EARLY_MORNING}}</t>
+  </si>
+  <si>
+    <t>{{extra_worked_days.sum.EARLY_MORNING}}</t>
   </si>
   <si>
     <t>les jours cochés correspondent à l'exécution des Prestations ( matin et aprés midi)</t>
@@ -308,7 +902,7 @@
     <numFmt numFmtId="165" formatCode="MMM\-YY"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -396,11 +990,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -909,7 +1498,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1008,8 +1597,8 @@
   </sheetPr>
   <dimension ref="A1:IW43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H38" activeCellId="0" sqref="H38"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95"/>
@@ -4941,38 +5530,102 @@
       <c r="B17" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="32"/>
-      <c r="Q17" s="32"/>
-      <c r="R17" s="32"/>
-      <c r="S17" s="32"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="32"/>
-      <c r="V17" s="32"/>
-      <c r="W17" s="32"/>
-      <c r="X17" s="32"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="32"/>
-      <c r="AC17" s="32"/>
-      <c r="AD17" s="32"/>
-      <c r="AE17" s="32"/>
-      <c r="AF17" s="32"/>
-      <c r="AG17" s="32"/>
-      <c r="AH17" s="32"/>
+      <c r="C17" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="H17" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="J17" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K17" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="L17" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="M17" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="P17" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q17" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="R17" s="32" t="s">
+        <v>96</v>
+      </c>
+      <c r="S17" s="32" t="s">
+        <v>97</v>
+      </c>
+      <c r="T17" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="U17" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="V17" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="W17" s="32" t="s">
+        <v>101</v>
+      </c>
+      <c r="X17" s="32" t="s">
+        <v>102</v>
+      </c>
+      <c r="Y17" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z17" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA17" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB17" s="32" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC17" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD17" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE17" s="32" t="s">
+        <v>109</v>
+      </c>
+      <c r="AF17" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG17" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="AH17" s="32" t="s">
+        <v>112</v>
+      </c>
       <c r="AI17" s="32"/>
       <c r="AJ17" s="32"/>
       <c r="AK17" s="32"/>
@@ -4985,7 +5638,9 @@
       <c r="AR17" s="32"/>
       <c r="AS17" s="32"/>
       <c r="AT17" s="34"/>
-      <c r="AU17" s="37"/>
+      <c r="AU17" s="37" t="s">
+        <v>113</v>
+      </c>
       <c r="AV17" s="0"/>
       <c r="AW17" s="0"/>
       <c r="AX17" s="0"/>
@@ -5200,40 +5855,104 @@
     <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="31"/>
       <c r="B18" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="32"/>
-      <c r="O18" s="32"/>
-      <c r="P18" s="32"/>
-      <c r="Q18" s="32"/>
-      <c r="R18" s="32"/>
-      <c r="S18" s="32"/>
-      <c r="T18" s="32"/>
-      <c r="U18" s="32"/>
-      <c r="V18" s="32"/>
-      <c r="W18" s="32"/>
-      <c r="X18" s="32"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="32"/>
-      <c r="AC18" s="32"/>
-      <c r="AD18" s="32"/>
-      <c r="AE18" s="32"/>
-      <c r="AF18" s="32"/>
-      <c r="AG18" s="32"/>
-      <c r="AH18" s="32"/>
+        <v>114</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="32" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="K18" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="L18" s="32" t="s">
+        <v>124</v>
+      </c>
+      <c r="M18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="N18" s="32" t="s">
+        <v>126</v>
+      </c>
+      <c r="O18" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="P18" s="32" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q18" s="32" t="s">
+        <v>129</v>
+      </c>
+      <c r="R18" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="S18" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="T18" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="U18" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="V18" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="W18" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="X18" s="32" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y18" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z18" s="32" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA18" s="32" t="s">
+        <v>139</v>
+      </c>
+      <c r="AB18" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC18" s="32" t="s">
+        <v>141</v>
+      </c>
+      <c r="AD18" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="AE18" s="32" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF18" s="32" t="s">
+        <v>144</v>
+      </c>
+      <c r="AG18" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="AH18" s="32" t="s">
+        <v>146</v>
+      </c>
       <c r="AI18" s="32"/>
       <c r="AJ18" s="32"/>
       <c r="AK18" s="32"/>
@@ -5246,7 +5965,9 @@
       <c r="AR18" s="32"/>
       <c r="AS18" s="32"/>
       <c r="AT18" s="34"/>
-      <c r="AU18" s="38"/>
+      <c r="AU18" s="38" t="s">
+        <v>147</v>
+      </c>
       <c r="AV18" s="0"/>
       <c r="AW18" s="0"/>
       <c r="AX18" s="0"/>
@@ -5510,7 +6231,7 @@
     <row r="20" s="42" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="39"/>
       <c r="B20" s="40" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="C20" s="40"/>
       <c r="D20" s="40"/>
@@ -5661,7 +6382,7 @@
         <v>12</v>
       </c>
       <c r="B23" s="43" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="C23" s="43"/>
       <c r="D23" s="43"/>
@@ -6295,7 +7016,7 @@
     </row>
     <row r="26" s="36" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="44" t="s">
-        <v>84</v>
+        <v>150</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>47</v>
@@ -6415,38 +7136,102 @@
       <c r="B27" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="C27" s="32"/>
-      <c r="D27" s="32"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-      <c r="M27" s="32"/>
-      <c r="N27" s="32"/>
-      <c r="O27" s="32"/>
-      <c r="P27" s="32"/>
-      <c r="Q27" s="32"/>
-      <c r="R27" s="32"/>
-      <c r="S27" s="32"/>
-      <c r="T27" s="32"/>
-      <c r="U27" s="32"/>
-      <c r="V27" s="32"/>
-      <c r="W27" s="32"/>
-      <c r="X27" s="32"/>
-      <c r="Y27" s="32"/>
-      <c r="Z27" s="32"/>
-      <c r="AA27" s="32"/>
-      <c r="AB27" s="32"/>
-      <c r="AC27" s="32"/>
-      <c r="AD27" s="32"/>
-      <c r="AE27" s="32"/>
-      <c r="AF27" s="32"/>
-      <c r="AG27" s="32"/>
-      <c r="AH27" s="32"/>
+      <c r="C27" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="E27" s="32" t="s">
+        <v>153</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="G27" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="H27" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="I27" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="J27" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="K27" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="L27" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="M27" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="N27" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="O27" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="P27" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q27" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="R27" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="S27" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="T27" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="U27" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="V27" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="W27" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="X27" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y27" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="Z27" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="AA27" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB27" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC27" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD27" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="AE27" s="32" t="s">
+        <v>179</v>
+      </c>
+      <c r="AF27" s="32" t="s">
+        <v>180</v>
+      </c>
+      <c r="AG27" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="AH27" s="32" t="s">
+        <v>182</v>
+      </c>
       <c r="AI27" s="32"/>
       <c r="AJ27" s="32"/>
       <c r="AK27" s="32"/>
@@ -6459,8 +7244,8 @@
       <c r="AR27" s="32"/>
       <c r="AS27" s="32"/>
       <c r="AT27" s="34"/>
-      <c r="AU27" s="37" t="n">
-        <v>0</v>
+      <c r="AU27" s="37" t="s">
+        <v>183</v>
       </c>
       <c r="AV27" s="0"/>
       <c r="AW27" s="0"/>
@@ -6676,40 +7461,104 @@
     <row r="28" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="44"/>
       <c r="B28" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-      <c r="M28" s="32"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="32"/>
-      <c r="Q28" s="32"/>
-      <c r="R28" s="32"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="32"/>
-      <c r="U28" s="32"/>
-      <c r="V28" s="32"/>
-      <c r="W28" s="32"/>
-      <c r="X28" s="32"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="32"/>
-      <c r="AA28" s="32"/>
-      <c r="AB28" s="32"/>
-      <c r="AC28" s="32"/>
-      <c r="AD28" s="32"/>
-      <c r="AE28" s="32"/>
-      <c r="AF28" s="32"/>
-      <c r="AG28" s="32"/>
-      <c r="AH28" s="32"/>
+        <v>114</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>184</v>
+      </c>
+      <c r="D28" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>186</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>188</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="K28" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="L28" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>194</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>195</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>196</v>
+      </c>
+      <c r="P28" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="Q28" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="R28" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="S28" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="T28" s="32" t="s">
+        <v>201</v>
+      </c>
+      <c r="U28" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="V28" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="W28" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="X28" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y28" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z28" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="AA28" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="AB28" s="32" t="s">
+        <v>209</v>
+      </c>
+      <c r="AC28" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="AD28" s="32" t="s">
+        <v>211</v>
+      </c>
+      <c r="AE28" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="AF28" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="AG28" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="AH28" s="32" t="s">
+        <v>215</v>
+      </c>
       <c r="AI28" s="32"/>
       <c r="AJ28" s="32"/>
       <c r="AK28" s="32"/>
@@ -6722,8 +7571,8 @@
       <c r="AR28" s="32"/>
       <c r="AS28" s="32"/>
       <c r="AT28" s="34"/>
-      <c r="AU28" s="38" t="n">
-        <v>0</v>
+      <c r="AU28" s="32" t="s">
+        <v>216</v>
       </c>
       <c r="AV28" s="0"/>
       <c r="AW28" s="0"/>
@@ -6938,43 +7787,107 @@
     </row>
     <row r="29" s="42" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="44" t="s">
-        <v>85</v>
+        <v>217</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-      <c r="M29" s="32"/>
-      <c r="N29" s="32"/>
-      <c r="O29" s="32"/>
-      <c r="P29" s="32"/>
-      <c r="Q29" s="32"/>
-      <c r="R29" s="32"/>
-      <c r="S29" s="32"/>
-      <c r="T29" s="32"/>
-      <c r="U29" s="32"/>
-      <c r="V29" s="32"/>
-      <c r="W29" s="32"/>
-      <c r="X29" s="32"/>
-      <c r="Y29" s="32"/>
-      <c r="Z29" s="32"/>
-      <c r="AA29" s="32"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
-      <c r="AE29" s="32"/>
-      <c r="AF29" s="32"/>
-      <c r="AG29" s="32"/>
-      <c r="AH29" s="32"/>
+        <v>218</v>
+      </c>
+      <c r="C29" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="G29" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>224</v>
+      </c>
+      <c r="I29" s="32" t="s">
+        <v>225</v>
+      </c>
+      <c r="J29" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>227</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>228</v>
+      </c>
+      <c r="M29" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="N29" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="O29" s="32" t="s">
+        <v>231</v>
+      </c>
+      <c r="P29" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q29" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="R29" s="32" t="s">
+        <v>234</v>
+      </c>
+      <c r="S29" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="T29" s="32" t="s">
+        <v>236</v>
+      </c>
+      <c r="U29" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="V29" s="32" t="s">
+        <v>238</v>
+      </c>
+      <c r="W29" s="32" t="s">
+        <v>239</v>
+      </c>
+      <c r="X29" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="Y29" s="32" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z29" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="AA29" s="32" t="s">
+        <v>243</v>
+      </c>
+      <c r="AB29" s="32" t="s">
+        <v>244</v>
+      </c>
+      <c r="AC29" s="32" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD29" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="AE29" s="32" t="s">
+        <v>247</v>
+      </c>
+      <c r="AF29" s="32" t="s">
+        <v>248</v>
+      </c>
+      <c r="AG29" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="AH29" s="32" t="s">
+        <v>250</v>
+      </c>
       <c r="AI29" s="32"/>
       <c r="AJ29" s="32"/>
       <c r="AK29" s="32"/>
@@ -6987,47 +7900,111 @@
       <c r="AR29" s="32"/>
       <c r="AS29" s="32"/>
       <c r="AT29" s="40"/>
-      <c r="AU29" s="37" t="n">
-        <v>0</v>
+      <c r="AU29" s="32" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="44"/>
       <c r="B30" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" s="32"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
-      <c r="O30" s="32"/>
-      <c r="P30" s="32"/>
-      <c r="Q30" s="32"/>
-      <c r="R30" s="32"/>
-      <c r="S30" s="32"/>
-      <c r="T30" s="32"/>
-      <c r="U30" s="32"/>
-      <c r="V30" s="32"/>
-      <c r="W30" s="32"/>
-      <c r="X30" s="32"/>
-      <c r="Y30" s="32"/>
-      <c r="Z30" s="32"/>
-      <c r="AA30" s="32"/>
-      <c r="AB30" s="32"/>
-      <c r="AC30" s="32"/>
-      <c r="AD30" s="32"/>
-      <c r="AE30" s="32"/>
-      <c r="AF30" s="32"/>
-      <c r="AG30" s="32"/>
-      <c r="AH30" s="32"/>
+        <v>252</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>253</v>
+      </c>
+      <c r="D30" s="32" t="s">
+        <v>254</v>
+      </c>
+      <c r="E30" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>256</v>
+      </c>
+      <c r="G30" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="H30" s="32" t="s">
+        <v>258</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="J30" s="32" t="s">
+        <v>260</v>
+      </c>
+      <c r="K30" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="L30" s="32" t="s">
+        <v>262</v>
+      </c>
+      <c r="M30" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="N30" s="32" t="s">
+        <v>264</v>
+      </c>
+      <c r="O30" s="32" t="s">
+        <v>265</v>
+      </c>
+      <c r="P30" s="32" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q30" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="R30" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="S30" s="32" t="s">
+        <v>269</v>
+      </c>
+      <c r="T30" s="32" t="s">
+        <v>270</v>
+      </c>
+      <c r="U30" s="32" t="s">
+        <v>271</v>
+      </c>
+      <c r="V30" s="32" t="s">
+        <v>272</v>
+      </c>
+      <c r="W30" s="32" t="s">
+        <v>273</v>
+      </c>
+      <c r="X30" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="Y30" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z30" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="AA30" s="32" t="s">
+        <v>277</v>
+      </c>
+      <c r="AB30" s="32" t="s">
+        <v>278</v>
+      </c>
+      <c r="AC30" s="32" t="s">
+        <v>279</v>
+      </c>
+      <c r="AD30" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="AE30" s="32" t="s">
+        <v>281</v>
+      </c>
+      <c r="AF30" s="32" t="s">
+        <v>282</v>
+      </c>
+      <c r="AG30" s="32" t="s">
+        <v>283</v>
+      </c>
+      <c r="AH30" s="32" t="s">
+        <v>284</v>
+      </c>
       <c r="AI30" s="32"/>
       <c r="AJ30" s="32"/>
       <c r="AK30" s="32"/>
@@ -7040,8 +8017,8 @@
       <c r="AR30" s="32"/>
       <c r="AS30" s="32"/>
       <c r="AT30" s="40"/>
-      <c r="AU30" s="38" t="n">
-        <v>0</v>
+      <c r="AU30" s="32" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7096,7 +8073,7 @@
     <row r="32" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="39"/>
       <c r="B32" s="45" t="s">
-        <v>88</v>
+        <v>286</v>
       </c>
       <c r="C32" s="45"/>
       <c r="D32" s="45"/>
@@ -7195,7 +8172,7 @@
     </row>
     <row r="34" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="39" t="s">
-        <v>89</v>
+        <v>287</v>
       </c>
       <c r="B34" s="46"/>
       <c r="C34" s="46"/>
@@ -7351,7 +8328,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="49" t="s">
-        <v>90</v>
+        <v>288</v>
       </c>
       <c r="I37" s="49"/>
       <c r="J37" s="49"/>
@@ -7396,7 +8373,7 @@
     <row r="38" customFormat="false" ht="41.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="9"/>
       <c r="B38" s="50" t="s">
-        <v>91</v>
+        <v>289</v>
       </c>
       <c r="C38" s="50"/>
       <c r="D38" s="50"/>
@@ -7404,7 +8381,7 @@
       <c r="F38" s="50"/>
       <c r="G38" s="50"/>
       <c r="H38" s="51" t="s">
-        <v>92</v>
+        <v>290</v>
       </c>
       <c r="I38" s="51"/>
       <c r="J38" s="51"/>
@@ -7595,7 +8572,7 @@
     </row>
     <row r="42" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="52" t="s">
-        <v>93</v>
+        <v>291</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>

</xml_diff>